<commit_message>
Medication Table and Incidents after V3
</commit_message>
<xml_diff>
--- a/Med2FreqPretty.xlsx
+++ b/Med2FreqPretty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\repositories\JHSGut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D980617D-7A08-4C9A-9762-57E89414D3CC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{920F0A86-F40F-483A-A21E-69E829849DD5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="0" windowWidth="16340" windowHeight="9360"/>
+    <workbookView xWindow="4500" yWindow="1380" windowWidth="21600" windowHeight="11265"/>
   </bookViews>
   <sheets>
     <sheet name="Med2Freq" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>n</t>
+  </si>
   <si>
     <t>ANTIHYPERTENSIVES</t>
   </si>
@@ -28,43 +31,43 @@
     <t>ANALGESICS - NONNARCOTIC</t>
   </si>
   <si>
+    <t>ANTIHYPERLIPIDEMICS</t>
+  </si>
+  <si>
     <t>MULTIVITAMINS</t>
   </si>
   <si>
-    <t>ANTIHYPERLIPIDEMICS</t>
+    <t>DIURETICS</t>
+  </si>
+  <si>
+    <t>CALCIUM CHANNEL BLOCKERS</t>
   </si>
   <si>
     <t>ANTIDIABETICS</t>
   </si>
   <si>
-    <t>DIURETICS</t>
-  </si>
-  <si>
     <t>MINERALS &amp; ELECTROLYTES</t>
   </si>
   <si>
-    <t>CALCIUM CHANNEL BLOCKERS</t>
+    <t>ANALGESICS - ANTI-INFLAMMATORY</t>
+  </si>
+  <si>
+    <t>BETA BLOCKERS</t>
+  </si>
+  <si>
+    <t>ULCER DRUGS</t>
   </si>
   <si>
     <t>VITAMINS</t>
   </si>
   <si>
-    <t>ANALGESICS - ANTI-INFLAMMATORY</t>
-  </si>
-  <si>
-    <t>ULCER DRUGS</t>
-  </si>
-  <si>
-    <t>BETA BLOCKERS</t>
-  </si>
-  <si>
     <t>Medication Class</t>
   </si>
   <si>
     <t>Classification Code</t>
   </si>
   <si>
-    <t>Frequency</t>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -577,8 +580,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -621,61 +625,80 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -987,158 +1010,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" customWidth="1"/>
-    <col min="3" max="3" width="10.36328125" customWidth="1"/>
+    <col min="1" max="1" width="33.6328125" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>3600000000</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1908</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>6400000000</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1719</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3900000000</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1277</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>7800000000</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1207</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3700000000</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1052</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3400000000</v>
+      </c>
+      <c r="C7" s="2">
+        <v>887</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2700000000</v>
+      </c>
+      <c r="C8" s="2">
+        <v>884</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>7900000000</v>
+      </c>
+      <c r="C9" s="2">
+        <v>875</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>6600000000</v>
+      </c>
+      <c r="C10" s="2">
+        <v>775</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>3300000000</v>
+      </c>
+      <c r="C11" s="2">
+        <v>711</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4900000000</v>
+      </c>
+      <c r="C12" s="2">
+        <v>677</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>3600000000</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>6400000000</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1842</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>7800000000</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1353</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>3900000000</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1331</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2700000000</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1287</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3700000000</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7900000000</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
-        <v>3400000000</v>
-      </c>
-      <c r="C9" s="1">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="B13" s="2">
         <v>7700000000</v>
       </c>
-      <c r="C10" s="1">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1">
-        <v>6600000000</v>
-      </c>
-      <c r="C11" s="1">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1">
-        <v>4900000000</v>
-      </c>
-      <c r="C12" s="1">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1">
-        <v>3300000000</v>
-      </c>
-      <c r="C13" s="1">
-        <v>719</v>
+      <c r="C13" s="2">
+        <v>638</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>